<commit_message>
calculo de conversion promedio
</commit_message>
<xml_diff>
--- a/doc/E4/3Workers/mpstatworkercpuusage.xlsx
+++ b/doc/E4/3Workers/mpstatworkercpuusage.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CursosCodigo\Proyecto-Grupo16-202120\doc\E4\3Workers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76A0190D-4C86-4A7A-A290-727BD9E994C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60EDCF0-4D86-486E-9D4E-BA26A30E5982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{305C0D28-133E-4CB0-8293-07DC9AE3364E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{305C0D28-133E-4CB0-8293-07DC9AE3364E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Uso de CPU" sheetId="1" r:id="rId1"/>
+    <sheet name="TiempoConversion" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="26">
   <si>
     <t xml:space="preserve">Linux 5.3.0-1033-aws (ip-172-31-18-79) </t>
   </si>
@@ -87,6 +88,30 @@
   <si>
     <t>Porcentaje promedio de sistema sin utilizar</t>
   </si>
+  <si>
+    <t>Worker 1</t>
+  </si>
+  <si>
+    <t>Tiempos de conversión muestreo</t>
+  </si>
+  <si>
+    <t>Worker 2</t>
+  </si>
+  <si>
+    <t>Worker 3</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>seg/min</t>
+  </si>
+  <si>
+    <t>Workers</t>
+  </si>
+  <si>
+    <t>Peticiones/worker</t>
+  </si>
 </sst>
 </file>
 
@@ -121,9 +146,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3AAB3E-65D6-45CC-BAB8-989939446E69}">
   <dimension ref="A1:M105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="S101" sqref="S101"/>
     </sheetView>
   </sheetViews>
@@ -4348,4 +4376,188 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2C6A63-D557-41BB-9947-9DAA0F3F5065}">
+  <dimension ref="B1:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2">
+        <v>60</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3.5350000000000001</v>
+      </c>
+      <c r="C4">
+        <v>3.706</v>
+      </c>
+      <c r="D4">
+        <v>3.5190000000000001</v>
+      </c>
+      <c r="G4">
+        <f>G2*G1/F14</f>
+        <v>166.21275619283549</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3.202</v>
+      </c>
+      <c r="C5">
+        <v>4.7510000000000003</v>
+      </c>
+      <c r="D5">
+        <v>3.4769999999999999</v>
+      </c>
+      <c r="G5">
+        <f>G3*G2*G1/F14</f>
+        <v>498.63826857850643</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>3.2829999999999999</v>
+      </c>
+      <c r="C6">
+        <v>3.41</v>
+      </c>
+      <c r="D6">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3.3940000000000001</v>
+      </c>
+      <c r="C7">
+        <v>3.63</v>
+      </c>
+      <c r="D7">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3.89</v>
+      </c>
+      <c r="C8">
+        <v>3.6110000000000002</v>
+      </c>
+      <c r="D8">
+        <v>3.5539999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3.516</v>
+      </c>
+      <c r="C9">
+        <v>3.9329999999999998</v>
+      </c>
+      <c r="D9">
+        <v>3.4710000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3.38</v>
+      </c>
+      <c r="C10">
+        <v>3.7490000000000001</v>
+      </c>
+      <c r="D10">
+        <v>3.339</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>3.5379999999999998</v>
+      </c>
+      <c r="C11">
+        <v>3.5880000000000001</v>
+      </c>
+      <c r="D11">
+        <v>3.4729999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>3.3879999999999999</v>
+      </c>
+      <c r="C12">
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="D12">
+        <v>3.4889999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f>GEOMEAN(B4:B12)</f>
+        <v>3.4535660211169428</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:D14" si="0">GEOMEAN(C4:C12)</f>
+        <v>3.7562081012553246</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>3.6261293320899721</v>
+      </c>
+      <c r="F14">
+        <f>GEOMEAN(B14:D14)</f>
+        <v>3.6098312412550122</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>